<commit_message>
Refactor main server structure, updated services
- Reorganized main server folder structure (init, config, models, routes, services)
- Added CRUD and reporting services with consistent model/schema handling
- Removed old server files and unused model (.keras)
- Updated requirements.txt
- Updated synthetic data generators and regenerated datasets
</commit_message>
<xml_diff>
--- a/synthetic-data/synDatasets/port_tariffs.xlsx
+++ b/synthetic-data/synDatasets/port_tariffs.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
   <si>
-    <t>Port_Name</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Handling_Cost_(₹/tonne)</t>
-  </si>
-  <si>
-    <t>Storage_Cost_(₹/tonne/day)</t>
-  </si>
-  <si>
-    <t>Max_Throughput_T/Day</t>
+    <t>port_name</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>handling_cost_inr_tonne</t>
+  </si>
+  <si>
+    <t>storage_cost_inr_tonne_day</t>
+  </si>
+  <si>
+    <t>max_throughput_t_day</t>
   </si>
   <si>
     <t>Haldia Port</t>
@@ -445,13 +445,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>351.52</v>
+        <v>213.48</v>
       </c>
       <c r="D2" s="1">
-        <v>9.880000000000001</v>
+        <v>11.6</v>
       </c>
       <c r="E2" s="1">
-        <v>24700</v>
+        <v>26900</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -462,13 +462,13 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <v>170.8</v>
+        <v>197.44</v>
       </c>
       <c r="D3" s="1">
-        <v>6.33</v>
+        <v>7.45</v>
       </c>
       <c r="E3" s="1">
-        <v>19400</v>
+        <v>20300</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -479,13 +479,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <v>324.27</v>
+        <v>303.12</v>
       </c>
       <c r="D4" s="1">
-        <v>11.53</v>
+        <v>13.06</v>
       </c>
       <c r="E4" s="1">
-        <v>18000</v>
+        <v>11900</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -496,13 +496,13 @@
         <v>9</v>
       </c>
       <c r="C5" s="1">
-        <v>236.99</v>
+        <v>318.08</v>
       </c>
       <c r="D5" s="1">
-        <v>9.529999999999999</v>
+        <v>9.57</v>
       </c>
       <c r="E5" s="1">
-        <v>20300</v>
+        <v>22800</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -513,13 +513,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <v>214.57</v>
+        <v>260.67</v>
       </c>
       <c r="D6" s="1">
-        <v>4.87</v>
+        <v>5.95</v>
       </c>
       <c r="E6" s="1">
-        <v>23400</v>
+        <v>17400</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -530,13 +530,13 @@
         <v>11</v>
       </c>
       <c r="C7" s="1">
-        <v>306.49</v>
+        <v>291.21</v>
       </c>
       <c r="D7" s="1">
-        <v>13.4</v>
+        <v>11.83</v>
       </c>
       <c r="E7" s="1">
-        <v>16100</v>
+        <v>11800</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -547,13 +547,13 @@
         <v>9</v>
       </c>
       <c r="C8" s="1">
-        <v>250.19</v>
+        <v>332.47</v>
       </c>
       <c r="D8" s="1">
-        <v>8.710000000000001</v>
+        <v>9.619999999999999</v>
       </c>
       <c r="E8" s="1">
-        <v>21200</v>
+        <v>21100</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -564,10 +564,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>209.22</v>
+        <v>222.09</v>
       </c>
       <c r="D9" s="1">
-        <v>5.21</v>
+        <v>6.03</v>
       </c>
       <c r="E9" s="1">
         <v>18100</v>
@@ -581,13 +581,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="1">
-        <v>299.7</v>
+        <v>419.1</v>
       </c>
       <c r="D10" s="1">
-        <v>12.36</v>
+        <v>11.03</v>
       </c>
       <c r="E10" s="1">
-        <v>19100</v>
+        <v>13900</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -598,13 +598,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>280.19</v>
+        <v>235.36</v>
       </c>
       <c r="D11" s="1">
-        <v>10.07</v>
+        <v>10.51</v>
       </c>
       <c r="E11" s="1">
-        <v>21000</v>
+        <v>21900</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -615,13 +615,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>258.86</v>
+        <v>210.42</v>
       </c>
       <c r="D12" s="1">
-        <v>5.4</v>
+        <v>5.35</v>
       </c>
       <c r="E12" s="1">
-        <v>23900</v>
+        <v>16600</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -632,13 +632,13 @@
         <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>391.94</v>
+        <v>376.55</v>
       </c>
       <c r="D13" s="1">
-        <v>12.55</v>
+        <v>14.96</v>
       </c>
       <c r="E13" s="1">
-        <v>16100</v>
+        <v>17000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>